<commit_message>
updating with channel by channel analysis results
</commit_message>
<xml_diff>
--- a/Python/2. Data Processing/2. Data Analysis/more_indepth_analysis.xlsx
+++ b/Python/2. Data Processing/2. Data Analysis/more_indepth_analysis.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sensata2com-my.sharepoint.com/personal/sofithcheallaigh_sensata_com/Documents/Desktop/Temp Git/masters_project/Python/2. Data Processing/2. Data Analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Courses\UUJ\Research Project\masters_project\Python\2. Data Processing\2. Data Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="93" documentId="13_ncr:1_{7A189A81-F773-4EC6-A608-C0A1BE673CD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C5251BA-E27F-49D6-B771-340C63210AB0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{129DF392-132C-4BB6-B74C-A26768156920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{524EAA27-FD1F-4B80-A5C4-579C1FDE3B36}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{524EAA27-FD1F-4B80-A5C4-579C1FDE3B36}"/>
   </bookViews>
   <sheets>
     <sheet name="Binary Analysis" sheetId="2" r:id="rId1"/>
     <sheet name="Grid Analysis" sheetId="1" r:id="rId2"/>
     <sheet name="Binary MovingAverage" sheetId="3" r:id="rId3"/>
+    <sheet name="Binary Channel Analysis" sheetId="4" r:id="rId4"/>
+    <sheet name="Multiclass Channel Analysis" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="27">
   <si>
     <t>Grid Wise Analysis</t>
   </si>
@@ -109,6 +111,15 @@
   <si>
     <t>Binary Analysis, where n = 10</t>
   </si>
+  <si>
+    <t>Binary Analysis, All Data Sets</t>
+  </si>
+  <si>
+    <t>Ch1</t>
+  </si>
+  <si>
+    <t>Ch2</t>
+  </si>
 </sst>
 </file>
 
@@ -123,7 +134,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -136,8 +147,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -285,11 +302,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -337,6 +380,31 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -829,6 +897,480 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>217170</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>26670</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>3810</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>194310</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Right Brace 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0775B985-1259-41B6-A80E-05DEE9ABC4C7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5017770" y="2550795"/>
+          <a:ext cx="396240" cy="1529715"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>217170</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>3810</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Right Brace 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{755931DD-7284-41F7-A64D-BCC4A9B7B316}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5017770" y="4295775"/>
+          <a:ext cx="396240" cy="1529715"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>243840</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Right Brace 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21E6036F-8021-4205-9A2F-8B7AABE0CD7A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13540740" y="2541270"/>
+          <a:ext cx="243840" cy="1529715"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>192405</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>417195</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>186690</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Right Brace 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A2CDFAE-9C2D-44BD-AD32-3841415F6B87}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13489305" y="4314825"/>
+          <a:ext cx="224790" cy="1529715"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>217170</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>26670</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>3810</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>194310</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Right Brace 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F84FF4A0-7AF1-4ABA-A34D-1D8F77D49670}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5017770" y="2560320"/>
+          <a:ext cx="396240" cy="1529715"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>217170</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>3810</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Right Brace 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3FAE6B6-7979-4EEF-B287-8D39E87F36B4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5017770" y="4295775"/>
+          <a:ext cx="396240" cy="1529715"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>243840</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Right Brace 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3AE49EF8-5EBB-457E-83DD-EDAAE730F6C1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13540740" y="2541270"/>
+          <a:ext cx="243840" cy="1529715"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>192405</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>417195</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>186690</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Right Brace 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70489F07-12EC-46FE-8EBF-04C2D6F848C8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13489305" y="4314825"/>
+          <a:ext cx="224790" cy="1529715"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1128,25 +1670,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F312B6F-D23A-4C1B-8D4A-809BAA3BCB29}">
   <dimension ref="B2:P29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:T29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="15" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="16"/>
       <c r="D3" s="17"/>
     </row>
-    <row r="4" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="11" t="s">
         <v>1</v>
       </c>
@@ -1155,7 +1697,7 @@
       </c>
       <c r="D4" s="14"/>
     </row>
-    <row r="5" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="12"/>
       <c r="C5" s="1" t="s">
         <v>2</v>
@@ -1164,7 +1706,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1175,7 +1717,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
@@ -1186,7 +1728,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
@@ -1197,7 +1739,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
@@ -1208,7 +1750,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
         <v>8</v>
       </c>
@@ -1219,8 +1761,8 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="15" t="s">
         <v>18</v>
       </c>
@@ -1232,7 +1774,7 @@
       <c r="M13" s="16"/>
       <c r="N13" s="17"/>
     </row>
-    <row r="14" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="11" t="s">
         <v>1</v>
       </c>
@@ -1246,7 +1788,7 @@
       </c>
       <c r="N14" s="14"/>
     </row>
-    <row r="15" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="12"/>
       <c r="C15" s="1" t="s">
         <v>2</v>
@@ -1262,7 +1804,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>4</v>
       </c>
@@ -1288,7 +1830,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>5</v>
       </c>
@@ -1314,7 +1856,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>6</v>
       </c>
@@ -1334,7 +1876,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>7</v>
       </c>
@@ -1354,7 +1896,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
         <v>8</v>
       </c>
@@ -1374,8 +1916,8 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="22" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="15" t="s">
         <v>18</v>
       </c>
@@ -1387,7 +1929,7 @@
       <c r="M22" s="16"/>
       <c r="N22" s="17"/>
     </row>
-    <row r="23" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="11" t="s">
         <v>1</v>
       </c>
@@ -1403,7 +1945,7 @@
       </c>
       <c r="N23" s="14"/>
     </row>
-    <row r="24" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="12"/>
       <c r="C24" s="1" t="s">
         <v>2</v>
@@ -1419,7 +1961,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
         <v>4</v>
       </c>
@@ -1445,7 +1987,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
         <v>5</v>
       </c>
@@ -1471,7 +2013,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
         <v>6</v>
       </c>
@@ -1491,7 +2033,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>7</v>
       </c>
@@ -1511,7 +2053,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="5" t="s">
         <v>8</v>
       </c>
@@ -1533,6 +2075,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="L22:N22"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="L23:L24"/>
+    <mergeCell ref="M23:N23"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="L14:L15"/>
@@ -1542,12 +2090,6 @@
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="L13:N13"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="L22:N22"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="L23:L24"/>
-    <mergeCell ref="M23:N23"/>
   </mergeCells>
   <conditionalFormatting sqref="C6:D10">
     <cfRule type="colorScale" priority="5">
@@ -1622,21 +2164,21 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="15" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="16"/>
       <c r="D3" s="17"/>
     </row>
-    <row r="4" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="11" t="s">
         <v>1</v>
       </c>
@@ -1645,7 +2187,7 @@
       </c>
       <c r="D4" s="14"/>
     </row>
-    <row r="5" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="12"/>
       <c r="C5" s="1" t="s">
         <v>2</v>
@@ -1660,7 +2202,7 @@
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1677,7 +2219,7 @@
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
@@ -1694,7 +2236,7 @@
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
@@ -1711,7 +2253,7 @@
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
@@ -1728,7 +2270,7 @@
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
     </row>
-    <row r="10" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
         <v>8</v>
       </c>
@@ -1745,8 +2287,8 @@
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
     </row>
-    <row r="12" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="15" t="s">
         <v>0</v>
       </c>
@@ -1758,7 +2300,7 @@
       <c r="M13" s="16"/>
       <c r="N13" s="17"/>
     </row>
-    <row r="14" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="11" t="s">
         <v>1</v>
       </c>
@@ -1772,7 +2314,7 @@
       </c>
       <c r="N14" s="14"/>
     </row>
-    <row r="15" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="12"/>
       <c r="C15" s="1" t="s">
         <v>2</v>
@@ -1788,7 +2330,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>4</v>
       </c>
@@ -1814,7 +2356,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>5</v>
       </c>
@@ -1840,7 +2382,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>6</v>
       </c>
@@ -1860,7 +2402,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>7</v>
       </c>
@@ -1880,7 +2422,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
         <v>8</v>
       </c>
@@ -1900,8 +2442,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="22" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="15" t="s">
         <v>0</v>
       </c>
@@ -1913,7 +2455,7 @@
       <c r="M22" s="16"/>
       <c r="N22" s="17"/>
     </row>
-    <row r="23" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="11" t="s">
         <v>1</v>
       </c>
@@ -1929,7 +2471,7 @@
       </c>
       <c r="N23" s="14"/>
     </row>
-    <row r="24" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="12"/>
       <c r="C24" s="1" t="s">
         <v>2</v>
@@ -1945,7 +2487,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
         <v>4</v>
       </c>
@@ -1971,7 +2513,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
         <v>5</v>
       </c>
@@ -1997,7 +2539,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
         <v>6</v>
       </c>
@@ -2017,7 +2559,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>7</v>
       </c>
@@ -2037,7 +2579,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="5" t="s">
         <v>8</v>
       </c>
@@ -2059,6 +2601,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:D14"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="B23:B24"/>
     <mergeCell ref="C23:D23"/>
@@ -2068,12 +2616,6 @@
     <mergeCell ref="L22:N22"/>
     <mergeCell ref="L23:L24"/>
     <mergeCell ref="M23:N23"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:D14"/>
   </mergeCells>
   <conditionalFormatting sqref="C6:D10">
     <cfRule type="colorScale" priority="5">
@@ -2145,20 +2687,20 @@
   <dimension ref="B2:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B3" sqref="B3:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="24.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="15" t="s">
         <v>23</v>
       </c>
@@ -2175,7 +2717,7 @@
       <c r="K3" s="16"/>
       <c r="L3" s="17"/>
     </row>
-    <row r="4" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="11" t="s">
         <v>1</v>
       </c>
@@ -2198,7 +2740,7 @@
       </c>
       <c r="L4" s="14"/>
     </row>
-    <row r="5" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="12"/>
       <c r="C5" s="1" t="s">
         <v>2</v>
@@ -2221,7 +2763,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
@@ -2250,7 +2792,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
@@ -2279,7 +2821,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
@@ -2308,7 +2850,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
@@ -2337,7 +2879,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
         <v>8</v>
       </c>
@@ -2366,8 +2908,8 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="15" t="s">
         <v>20</v>
       </c>
@@ -2384,7 +2926,7 @@
       <c r="K14" s="16"/>
       <c r="L14" s="17"/>
     </row>
-    <row r="15" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="11" t="s">
         <v>1</v>
       </c>
@@ -2407,7 +2949,7 @@
       </c>
       <c r="L15" s="14"/>
     </row>
-    <row r="16" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="12"/>
       <c r="C16" s="1" t="s">
         <v>2</v>
@@ -2430,7 +2972,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>4</v>
       </c>
@@ -2459,7 +3001,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>5</v>
       </c>
@@ -2488,7 +3030,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>6</v>
       </c>
@@ -2517,7 +3059,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>7</v>
       </c>
@@ -2546,7 +3088,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="5" t="s">
         <v>8</v>
       </c>
@@ -2577,24 +3119,24 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="K4:L4"/>
     <mergeCell ref="F3:H3"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:D4"/>
-    <mergeCell ref="J14:L14"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:D15"/>
   </mergeCells>
   <conditionalFormatting sqref="G17:H21">
     <cfRule type="colorScale" priority="6">
@@ -2670,4 +3212,2962 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{792366D3-1D0D-497C-9C39-4BE4DD4E20E9}">
+  <dimension ref="A2:Y53"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" customWidth="1"/>
+    <col min="14" max="14" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="21"/>
+    </row>
+    <row r="4" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="14"/>
+      <c r="E4" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="14"/>
+    </row>
+    <row r="5" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="12"/>
+      <c r="C5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="8">
+        <v>91</v>
+      </c>
+      <c r="D6" s="4">
+        <v>91</v>
+      </c>
+      <c r="E6" s="8">
+        <v>87</v>
+      </c>
+      <c r="F6" s="4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="9">
+        <v>99</v>
+      </c>
+      <c r="D7" s="4">
+        <v>99</v>
+      </c>
+      <c r="E7" s="9">
+        <v>99</v>
+      </c>
+      <c r="F7" s="4">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="9">
+        <v>99</v>
+      </c>
+      <c r="D8" s="4">
+        <v>99</v>
+      </c>
+      <c r="E8" s="9">
+        <v>99</v>
+      </c>
+      <c r="F8" s="4">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="9">
+        <v>92</v>
+      </c>
+      <c r="D9" s="4">
+        <v>92</v>
+      </c>
+      <c r="E9" s="9">
+        <v>88</v>
+      </c>
+      <c r="F9" s="4">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="10">
+        <v>92</v>
+      </c>
+      <c r="D10" s="6">
+        <v>92</v>
+      </c>
+      <c r="E10" s="10">
+        <v>87</v>
+      </c>
+      <c r="F10" s="6">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="O14" s="20"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="20"/>
+      <c r="R14" s="21"/>
+      <c r="S14" s="18"/>
+      <c r="T14" s="18"/>
+      <c r="U14" s="18"/>
+      <c r="V14" s="18"/>
+    </row>
+    <row r="15" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="14"/>
+      <c r="E15" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="14"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="O15" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="R15" s="14"/>
+      <c r="S15" s="18"/>
+      <c r="T15" s="18"/>
+      <c r="U15" s="18"/>
+      <c r="V15" s="18"/>
+    </row>
+    <row r="16" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="28"/>
+      <c r="C16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
+      <c r="N16" s="28"/>
+      <c r="O16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="R16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="S16" s="18"/>
+      <c r="T16" s="18"/>
+      <c r="U16" s="18"/>
+      <c r="V16" s="18"/>
+      <c r="X16" s="18"/>
+      <c r="Y16" s="18"/>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B17" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="8">
+        <v>93</v>
+      </c>
+      <c r="D17" s="4">
+        <v>97</v>
+      </c>
+      <c r="E17" s="8">
+        <v>87</v>
+      </c>
+      <c r="F17" s="4">
+        <v>90</v>
+      </c>
+      <c r="H17" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="18"/>
+      <c r="N17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="O17" s="8">
+        <v>100</v>
+      </c>
+      <c r="P17" s="4">
+        <v>78</v>
+      </c>
+      <c r="Q17" s="8">
+        <v>100</v>
+      </c>
+      <c r="R17" s="4">
+        <v>54</v>
+      </c>
+      <c r="T17" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="U17" s="18"/>
+      <c r="V17" s="18"/>
+      <c r="W17" s="18"/>
+      <c r="X17" s="18"/>
+      <c r="Y17" s="18"/>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B18" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="9">
+        <v>99</v>
+      </c>
+      <c r="D18" s="4">
+        <v>95</v>
+      </c>
+      <c r="E18" s="9">
+        <v>99</v>
+      </c>
+      <c r="F18" s="4">
+        <v>97</v>
+      </c>
+      <c r="H18" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
+      <c r="M18" s="18"/>
+      <c r="N18" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O18" s="9">
+        <v>100</v>
+      </c>
+      <c r="P18" s="4">
+        <v>87</v>
+      </c>
+      <c r="Q18" s="9">
+        <v>100</v>
+      </c>
+      <c r="R18" s="4">
+        <v>54</v>
+      </c>
+      <c r="T18" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="U18" s="18"/>
+      <c r="V18" s="18"/>
+      <c r="W18" s="18"/>
+      <c r="X18" s="18"/>
+      <c r="Y18" s="18"/>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B19" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="9">
+        <v>99</v>
+      </c>
+      <c r="D19" s="4">
+        <v>95</v>
+      </c>
+      <c r="E19" s="9">
+        <v>99</v>
+      </c>
+      <c r="F19" s="4">
+        <v>97</v>
+      </c>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="18"/>
+      <c r="M19" s="18"/>
+      <c r="N19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="O19" s="9">
+        <v>100</v>
+      </c>
+      <c r="P19" s="4">
+        <v>90</v>
+      </c>
+      <c r="Q19" s="9">
+        <v>100</v>
+      </c>
+      <c r="R19" s="4">
+        <v>53</v>
+      </c>
+      <c r="S19" s="18"/>
+      <c r="X19" s="18"/>
+      <c r="Y19" s="18"/>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B20" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="9">
+        <v>91</v>
+      </c>
+      <c r="D20" s="4">
+        <v>97</v>
+      </c>
+      <c r="E20" s="9">
+        <v>89</v>
+      </c>
+      <c r="F20" s="4">
+        <v>92</v>
+      </c>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="O20" s="9">
+        <v>98</v>
+      </c>
+      <c r="P20" s="4">
+        <v>77</v>
+      </c>
+      <c r="Q20" s="9">
+        <v>98</v>
+      </c>
+      <c r="R20" s="4">
+        <v>58</v>
+      </c>
+      <c r="S20" s="18"/>
+      <c r="T20" s="18"/>
+      <c r="U20" s="18"/>
+      <c r="V20" s="18"/>
+      <c r="X20" s="18"/>
+      <c r="Y20" s="18"/>
+    </row>
+    <row r="21" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="10">
+        <v>90</v>
+      </c>
+      <c r="D21" s="6">
+        <v>97</v>
+      </c>
+      <c r="E21" s="10">
+        <v>86</v>
+      </c>
+      <c r="F21" s="6">
+        <v>83</v>
+      </c>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="O21" s="10">
+        <v>98</v>
+      </c>
+      <c r="P21" s="6">
+        <v>77</v>
+      </c>
+      <c r="Q21" s="10">
+        <v>98</v>
+      </c>
+      <c r="R21" s="6">
+        <v>58</v>
+      </c>
+      <c r="S21" s="18"/>
+      <c r="T21" s="18"/>
+      <c r="U21" s="18"/>
+      <c r="V21" s="18"/>
+    </row>
+    <row r="22" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="18"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="18"/>
+      <c r="N22" s="18"/>
+      <c r="O22" s="18"/>
+      <c r="P22" s="18"/>
+      <c r="Q22" s="18"/>
+      <c r="R22" s="18"/>
+      <c r="S22" s="18"/>
+      <c r="T22" s="18"/>
+      <c r="U22" s="18"/>
+      <c r="V22" s="18"/>
+    </row>
+    <row r="23" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="O23" s="20"/>
+      <c r="P23" s="20"/>
+      <c r="Q23" s="20"/>
+      <c r="R23" s="21"/>
+      <c r="S23" s="18"/>
+      <c r="T23" s="18"/>
+      <c r="U23" s="18"/>
+      <c r="V23" s="18"/>
+    </row>
+    <row r="24" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="14"/>
+      <c r="E24" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" s="14"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="O24" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="P24" s="14"/>
+      <c r="Q24" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="R24" s="14"/>
+      <c r="S24" s="18"/>
+      <c r="T24" s="18"/>
+      <c r="U24" s="18"/>
+      <c r="V24" s="18"/>
+    </row>
+    <row r="25" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="28"/>
+      <c r="C25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
+      <c r="M25" s="18"/>
+      <c r="N25" s="28"/>
+      <c r="O25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="R25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="S25" s="18"/>
+      <c r="T25" s="18"/>
+      <c r="U25" s="18"/>
+      <c r="V25" s="18"/>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="8">
+        <v>93</v>
+      </c>
+      <c r="D26" s="4">
+        <v>95</v>
+      </c>
+      <c r="E26" s="8">
+        <v>87</v>
+      </c>
+      <c r="F26" s="4">
+        <v>90</v>
+      </c>
+      <c r="H26" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="18"/>
+      <c r="N26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="O26" s="8">
+        <v>94</v>
+      </c>
+      <c r="P26" s="4">
+        <v>96</v>
+      </c>
+      <c r="Q26" s="8">
+        <v>87</v>
+      </c>
+      <c r="R26" s="4">
+        <v>90</v>
+      </c>
+      <c r="T26" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="U26" s="18"/>
+      <c r="V26" s="18"/>
+      <c r="W26" s="18"/>
+      <c r="X26" s="18"/>
+      <c r="Y26" s="18"/>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B27" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="9">
+        <v>99</v>
+      </c>
+      <c r="D27" s="4">
+        <v>96</v>
+      </c>
+      <c r="E27" s="9">
+        <v>99</v>
+      </c>
+      <c r="F27" s="4">
+        <v>98</v>
+      </c>
+      <c r="H27" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="18"/>
+      <c r="M27" s="18"/>
+      <c r="N27" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O27" s="9">
+        <v>99</v>
+      </c>
+      <c r="P27" s="4">
+        <v>95</v>
+      </c>
+      <c r="Q27" s="9">
+        <v>99</v>
+      </c>
+      <c r="R27" s="4">
+        <v>98</v>
+      </c>
+      <c r="T27" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="U27" s="18"/>
+      <c r="V27" s="18"/>
+      <c r="W27" s="18"/>
+      <c r="X27" s="18"/>
+      <c r="Y27" s="18"/>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="9">
+        <v>99</v>
+      </c>
+      <c r="D28" s="4">
+        <v>96</v>
+      </c>
+      <c r="E28" s="9">
+        <v>99</v>
+      </c>
+      <c r="F28" s="4">
+        <v>98</v>
+      </c>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="18"/>
+      <c r="M28" s="18"/>
+      <c r="N28" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="O28" s="9">
+        <v>99</v>
+      </c>
+      <c r="P28" s="4">
+        <v>95</v>
+      </c>
+      <c r="Q28" s="9">
+        <v>99</v>
+      </c>
+      <c r="R28" s="4">
+        <v>98</v>
+      </c>
+      <c r="S28" s="18"/>
+      <c r="T28" s="18"/>
+      <c r="U28" s="18"/>
+      <c r="V28" s="18"/>
+      <c r="X28" s="18"/>
+      <c r="Y28" s="18"/>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B29" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="9">
+        <v>91</v>
+      </c>
+      <c r="D29" s="4">
+        <v>95</v>
+      </c>
+      <c r="E29" s="9">
+        <v>89</v>
+      </c>
+      <c r="F29" s="4">
+        <v>92</v>
+      </c>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="18"/>
+      <c r="M29" s="18"/>
+      <c r="N29" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="O29" s="9">
+        <v>92</v>
+      </c>
+      <c r="P29" s="4">
+        <v>96</v>
+      </c>
+      <c r="Q29" s="9">
+        <v>89</v>
+      </c>
+      <c r="R29" s="4">
+        <v>92</v>
+      </c>
+      <c r="S29" s="18"/>
+      <c r="T29" s="18"/>
+      <c r="U29" s="18"/>
+      <c r="V29" s="18"/>
+    </row>
+    <row r="30" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="10">
+        <v>90</v>
+      </c>
+      <c r="D30" s="6">
+        <v>97</v>
+      </c>
+      <c r="E30" s="10">
+        <v>90</v>
+      </c>
+      <c r="F30" s="6">
+        <v>90</v>
+      </c>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="18"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="18"/>
+      <c r="M30" s="18"/>
+      <c r="N30" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="O30" s="10">
+        <v>90</v>
+      </c>
+      <c r="P30" s="6">
+        <v>97</v>
+      </c>
+      <c r="Q30" s="10">
+        <v>90</v>
+      </c>
+      <c r="R30" s="6">
+        <v>90</v>
+      </c>
+      <c r="S30" s="18"/>
+      <c r="T30" s="18"/>
+      <c r="U30" s="18"/>
+      <c r="V30" s="18"/>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="18"/>
+      <c r="L31" s="18"/>
+      <c r="M31" s="18"/>
+      <c r="N31" s="18"/>
+      <c r="O31" s="18"/>
+      <c r="P31" s="18"/>
+      <c r="Q31" s="18"/>
+      <c r="R31" s="18"/>
+      <c r="S31" s="18"/>
+      <c r="T31" s="18"/>
+      <c r="U31" s="18"/>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="18"/>
+      <c r="M32" s="18"/>
+      <c r="N32" s="18"/>
+      <c r="O32" s="18"/>
+      <c r="P32" s="18"/>
+      <c r="Q32" s="18"/>
+      <c r="R32" s="18"/>
+      <c r="S32" s="18"/>
+      <c r="T32" s="18"/>
+      <c r="U32" s="18"/>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A33" s="18"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="18"/>
+      <c r="M33" s="18"/>
+      <c r="N33" s="18"/>
+      <c r="O33" s="18"/>
+      <c r="P33" s="18"/>
+      <c r="Q33" s="18"/>
+      <c r="R33" s="18"/>
+      <c r="S33" s="18"/>
+      <c r="T33" s="18"/>
+      <c r="U33" s="18"/>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A34" s="18"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="18"/>
+      <c r="J34" s="18"/>
+      <c r="K34" s="18"/>
+      <c r="L34" s="18"/>
+      <c r="M34" s="18"/>
+      <c r="N34" s="18"/>
+      <c r="O34" s="18"/>
+      <c r="P34" s="18"/>
+      <c r="Q34" s="18"/>
+      <c r="R34" s="18"/>
+      <c r="S34" s="18"/>
+      <c r="T34" s="18"/>
+      <c r="U34" s="18"/>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A35" s="18"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="18"/>
+      <c r="I35" s="18"/>
+      <c r="J35" s="18"/>
+      <c r="K35" s="18"/>
+      <c r="L35" s="18"/>
+      <c r="M35" s="18"/>
+      <c r="N35" s="18"/>
+      <c r="O35" s="18"/>
+      <c r="P35" s="18"/>
+      <c r="Q35" s="18"/>
+      <c r="R35" s="18"/>
+      <c r="S35" s="18"/>
+      <c r="T35" s="18"/>
+      <c r="U35" s="18"/>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A36" s="18"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="18"/>
+      <c r="K36" s="18"/>
+      <c r="L36" s="18"/>
+      <c r="M36" s="18"/>
+      <c r="N36" s="18"/>
+      <c r="O36" s="18"/>
+      <c r="P36" s="18"/>
+      <c r="Q36" s="18"/>
+      <c r="R36" s="18"/>
+      <c r="S36" s="18"/>
+      <c r="T36" s="18"/>
+      <c r="U36" s="18"/>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A37" s="18"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="18"/>
+      <c r="J37" s="18"/>
+      <c r="K37" s="18"/>
+      <c r="L37" s="18"/>
+      <c r="M37" s="18"/>
+      <c r="N37" s="18"/>
+      <c r="O37" s="18"/>
+      <c r="P37" s="18"/>
+      <c r="Q37" s="18"/>
+      <c r="R37" s="18"/>
+      <c r="S37" s="18"/>
+      <c r="T37" s="18"/>
+      <c r="U37" s="18"/>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A38" s="18"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="18"/>
+      <c r="I38" s="18"/>
+      <c r="J38" s="18"/>
+      <c r="K38" s="18"/>
+      <c r="L38" s="18"/>
+      <c r="M38" s="18"/>
+      <c r="N38" s="18"/>
+      <c r="O38" s="18"/>
+      <c r="P38" s="18"/>
+      <c r="Q38" s="18"/>
+      <c r="R38" s="18"/>
+      <c r="S38" s="18"/>
+      <c r="T38" s="18"/>
+      <c r="U38" s="18"/>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A39" s="18"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="18"/>
+      <c r="I39" s="18"/>
+      <c r="J39" s="18"/>
+      <c r="K39" s="18"/>
+      <c r="L39" s="18"/>
+      <c r="M39" s="18"/>
+      <c r="N39" s="18"/>
+      <c r="O39" s="18"/>
+      <c r="P39" s="18"/>
+      <c r="Q39" s="18"/>
+      <c r="R39" s="18"/>
+      <c r="S39" s="18"/>
+      <c r="T39" s="18"/>
+      <c r="U39" s="18"/>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A40" s="18"/>
+      <c r="B40" s="18"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="18"/>
+      <c r="I40" s="18"/>
+      <c r="J40" s="18"/>
+      <c r="K40" s="18"/>
+      <c r="L40" s="18"/>
+      <c r="M40" s="18"/>
+      <c r="N40" s="18"/>
+      <c r="O40" s="18"/>
+      <c r="P40" s="18"/>
+      <c r="Q40" s="18"/>
+      <c r="R40" s="18"/>
+      <c r="S40" s="18"/>
+      <c r="T40" s="18"/>
+      <c r="U40" s="18"/>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A41" s="18"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="18"/>
+      <c r="I41" s="18"/>
+      <c r="J41" s="18"/>
+      <c r="K41" s="18"/>
+      <c r="L41" s="18"/>
+      <c r="M41" s="18"/>
+      <c r="N41" s="18"/>
+      <c r="O41" s="18"/>
+      <c r="P41" s="18"/>
+      <c r="Q41" s="18"/>
+      <c r="R41" s="18"/>
+      <c r="S41" s="18"/>
+      <c r="T41" s="18"/>
+      <c r="U41" s="18"/>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A42" s="18"/>
+      <c r="B42" s="18"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="18"/>
+      <c r="H42" s="18"/>
+      <c r="I42" s="18"/>
+      <c r="J42" s="18"/>
+      <c r="K42" s="18"/>
+      <c r="L42" s="18"/>
+      <c r="M42" s="18"/>
+      <c r="N42" s="18"/>
+      <c r="O42" s="18"/>
+      <c r="P42" s="18"/>
+      <c r="Q42" s="18"/>
+      <c r="R42" s="18"/>
+      <c r="S42" s="18"/>
+      <c r="T42" s="18"/>
+      <c r="U42" s="18"/>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A43" s="18"/>
+      <c r="B43" s="18"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="18"/>
+      <c r="G43" s="18"/>
+      <c r="H43" s="18"/>
+      <c r="I43" s="18"/>
+      <c r="J43" s="18"/>
+      <c r="K43" s="18"/>
+      <c r="L43" s="18"/>
+      <c r="M43" s="18"/>
+      <c r="N43" s="18"/>
+      <c r="O43" s="18"/>
+      <c r="P43" s="18"/>
+      <c r="Q43" s="18"/>
+      <c r="R43" s="18"/>
+      <c r="S43" s="18"/>
+      <c r="T43" s="18"/>
+      <c r="U43" s="18"/>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A44" s="18"/>
+      <c r="B44" s="18"/>
+      <c r="C44" s="26"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="18"/>
+      <c r="G44" s="18"/>
+      <c r="H44" s="18"/>
+      <c r="I44" s="18"/>
+      <c r="J44" s="18"/>
+      <c r="K44" s="18"/>
+      <c r="L44" s="18"/>
+      <c r="M44" s="18"/>
+      <c r="N44" s="18"/>
+      <c r="O44" s="18"/>
+      <c r="P44" s="18"/>
+      <c r="Q44" s="18"/>
+      <c r="R44" s="18"/>
+      <c r="S44" s="18"/>
+      <c r="T44" s="18"/>
+      <c r="U44" s="18"/>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A45" s="18"/>
+      <c r="B45" s="18"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="18"/>
+      <c r="H45" s="18"/>
+      <c r="I45" s="18"/>
+      <c r="J45" s="18"/>
+      <c r="K45" s="18"/>
+      <c r="L45" s="18"/>
+      <c r="M45" s="18"/>
+      <c r="N45" s="18"/>
+      <c r="O45" s="18"/>
+      <c r="P45" s="18"/>
+      <c r="Q45" s="18"/>
+      <c r="R45" s="18"/>
+      <c r="S45" s="18"/>
+      <c r="T45" s="18"/>
+      <c r="U45" s="18"/>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A46" s="18"/>
+      <c r="B46" s="18"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="18"/>
+      <c r="G46" s="18"/>
+      <c r="H46" s="18"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
+      <c r="K46" s="18"/>
+      <c r="L46" s="18"/>
+      <c r="M46" s="18"/>
+      <c r="N46" s="18"/>
+      <c r="O46" s="18"/>
+      <c r="P46" s="18"/>
+      <c r="Q46" s="18"/>
+      <c r="R46" s="18"/>
+      <c r="S46" s="18"/>
+      <c r="T46" s="18"/>
+      <c r="U46" s="18"/>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A47" s="18"/>
+      <c r="B47" s="18"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="18"/>
+      <c r="I47" s="18"/>
+      <c r="J47" s="18"/>
+      <c r="K47" s="18"/>
+      <c r="L47" s="18"/>
+      <c r="M47" s="18"/>
+      <c r="N47" s="18"/>
+      <c r="O47" s="18"/>
+      <c r="P47" s="18"/>
+      <c r="Q47" s="18"/>
+      <c r="R47" s="18"/>
+      <c r="S47" s="18"/>
+      <c r="T47" s="18"/>
+      <c r="U47" s="18"/>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A48" s="18"/>
+      <c r="B48" s="18"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
+      <c r="H48" s="18"/>
+      <c r="I48" s="18"/>
+      <c r="J48" s="18"/>
+      <c r="K48" s="18"/>
+      <c r="L48" s="18"/>
+      <c r="M48" s="18"/>
+      <c r="N48" s="18"/>
+      <c r="O48" s="18"/>
+      <c r="P48" s="18"/>
+      <c r="Q48" s="18"/>
+      <c r="R48" s="18"/>
+      <c r="S48" s="18"/>
+      <c r="T48" s="18"/>
+      <c r="U48" s="18"/>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A49" s="18"/>
+      <c r="B49" s="18"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="18"/>
+      <c r="G49" s="18"/>
+      <c r="H49" s="18"/>
+      <c r="I49" s="18"/>
+      <c r="J49" s="18"/>
+      <c r="K49" s="18"/>
+      <c r="L49" s="18"/>
+      <c r="M49" s="18"/>
+      <c r="N49" s="18"/>
+      <c r="O49" s="18"/>
+      <c r="P49" s="18"/>
+      <c r="Q49" s="18"/>
+      <c r="R49" s="18"/>
+      <c r="S49" s="18"/>
+      <c r="T49" s="18"/>
+      <c r="U49" s="18"/>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A50" s="18"/>
+      <c r="B50" s="18"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="18"/>
+      <c r="G50" s="18"/>
+      <c r="H50" s="18"/>
+      <c r="I50" s="18"/>
+      <c r="J50" s="18"/>
+      <c r="K50" s="18"/>
+      <c r="L50" s="18"/>
+      <c r="M50" s="18"/>
+      <c r="N50" s="18"/>
+      <c r="O50" s="18"/>
+      <c r="P50" s="18"/>
+      <c r="Q50" s="18"/>
+      <c r="R50" s="18"/>
+      <c r="S50" s="18"/>
+      <c r="T50" s="18"/>
+      <c r="U50" s="18"/>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A51" s="18"/>
+      <c r="B51" s="18"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="18"/>
+      <c r="G51" s="18"/>
+      <c r="H51" s="18"/>
+      <c r="I51" s="18"/>
+      <c r="J51" s="18"/>
+      <c r="K51" s="18"/>
+      <c r="L51" s="18"/>
+      <c r="M51" s="18"/>
+      <c r="N51" s="18"/>
+      <c r="O51" s="18"/>
+      <c r="P51" s="18"/>
+      <c r="Q51" s="18"/>
+      <c r="R51" s="18"/>
+      <c r="S51" s="18"/>
+      <c r="T51" s="18"/>
+      <c r="U51" s="18"/>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A52" s="18"/>
+      <c r="B52" s="18"/>
+      <c r="C52" s="18"/>
+      <c r="D52" s="18"/>
+      <c r="E52" s="18"/>
+      <c r="F52" s="18"/>
+      <c r="G52" s="18"/>
+      <c r="H52" s="18"/>
+      <c r="I52" s="18"/>
+      <c r="J52" s="18"/>
+      <c r="K52" s="18"/>
+      <c r="L52" s="18"/>
+      <c r="M52" s="18"/>
+      <c r="N52" s="18"/>
+      <c r="O52" s="18"/>
+      <c r="P52" s="18"/>
+      <c r="Q52" s="18"/>
+      <c r="R52" s="18"/>
+      <c r="S52" s="18"/>
+      <c r="T52" s="18"/>
+      <c r="U52" s="18"/>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B53" s="18"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="18"/>
+      <c r="I53" s="18"/>
+      <c r="J53" s="18"/>
+      <c r="K53" s="18"/>
+      <c r="L53" s="18"/>
+      <c r="M53" s="18"/>
+      <c r="N53" s="18"/>
+      <c r="O53" s="18"/>
+      <c r="P53" s="18"/>
+      <c r="Q53" s="18"/>
+      <c r="R53" s="18"/>
+      <c r="S53" s="18"/>
+      <c r="T53" s="18"/>
+      <c r="U53" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="24">
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="N24:N25"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="N23:R23"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="N15:N16"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="N14:R14"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="B3:F3"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C6:D10">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E6:F10">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C17:D21">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C26:D30">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O17:P21">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O26:P30">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E17:F21">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E26:F30">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q17:R21">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q26:R30">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4F528EF-5D62-48EC-8548-FEB5DDAD9EAE}">
+  <dimension ref="A2:Y53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" customWidth="1"/>
+    <col min="14" max="14" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="21"/>
+    </row>
+    <row r="4" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="14"/>
+      <c r="E4" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="14"/>
+    </row>
+    <row r="5" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="12"/>
+      <c r="C5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="6"/>
+    </row>
+    <row r="13" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="O14" s="20"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="20"/>
+      <c r="R14" s="21"/>
+      <c r="S14" s="18"/>
+      <c r="T14" s="18"/>
+      <c r="U14" s="18"/>
+      <c r="V14" s="18"/>
+    </row>
+    <row r="15" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="14"/>
+      <c r="E15" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="14"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="O15" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="R15" s="14"/>
+      <c r="S15" s="18"/>
+      <c r="T15" s="18"/>
+      <c r="U15" s="18"/>
+      <c r="V15" s="18"/>
+    </row>
+    <row r="16" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="28"/>
+      <c r="C16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
+      <c r="N16" s="28"/>
+      <c r="O16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="R16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="S16" s="18"/>
+      <c r="T16" s="18"/>
+      <c r="U16" s="18"/>
+      <c r="V16" s="18"/>
+      <c r="X16" s="18"/>
+      <c r="Y16" s="18"/>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B17" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="8">
+        <v>36</v>
+      </c>
+      <c r="D17" s="4">
+        <v>26</v>
+      </c>
+      <c r="E17" s="8">
+        <v>23</v>
+      </c>
+      <c r="F17" s="4">
+        <v>7</v>
+      </c>
+      <c r="H17" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="18"/>
+      <c r="N17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="O17" s="8">
+        <v>44</v>
+      </c>
+      <c r="P17" s="4">
+        <v>22</v>
+      </c>
+      <c r="Q17" s="8">
+        <v>40</v>
+      </c>
+      <c r="R17" s="4">
+        <v>20</v>
+      </c>
+      <c r="T17" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="U17" s="18"/>
+      <c r="V17" s="18"/>
+      <c r="W17" s="18"/>
+      <c r="X17" s="18"/>
+      <c r="Y17" s="18"/>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B18" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="9">
+        <v>97</v>
+      </c>
+      <c r="D18" s="4">
+        <v>18</v>
+      </c>
+      <c r="E18" s="9">
+        <v>97</v>
+      </c>
+      <c r="F18" s="4">
+        <v>25</v>
+      </c>
+      <c r="H18" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
+      <c r="M18" s="18"/>
+      <c r="N18" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O18" s="9">
+        <v>98</v>
+      </c>
+      <c r="P18" s="4">
+        <v>24</v>
+      </c>
+      <c r="Q18" s="9">
+        <v>98</v>
+      </c>
+      <c r="R18" s="4">
+        <v>12</v>
+      </c>
+      <c r="T18" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="U18" s="18"/>
+      <c r="V18" s="18"/>
+      <c r="W18" s="18"/>
+      <c r="X18" s="18"/>
+      <c r="Y18" s="18"/>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B19" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="9">
+        <v>96</v>
+      </c>
+      <c r="D19" s="4">
+        <v>16</v>
+      </c>
+      <c r="E19" s="9">
+        <v>96</v>
+      </c>
+      <c r="F19" s="4">
+        <v>20</v>
+      </c>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="18"/>
+      <c r="M19" s="18"/>
+      <c r="N19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="O19" s="9">
+        <v>98</v>
+      </c>
+      <c r="P19" s="4">
+        <v>25</v>
+      </c>
+      <c r="Q19" s="9">
+        <v>98</v>
+      </c>
+      <c r="R19" s="4">
+        <v>12</v>
+      </c>
+      <c r="S19" s="18"/>
+      <c r="X19" s="18"/>
+      <c r="Y19" s="18"/>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B20" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="9">
+        <v>37</v>
+      </c>
+      <c r="D20" s="4">
+        <v>38</v>
+      </c>
+      <c r="E20" s="9">
+        <v>24</v>
+      </c>
+      <c r="F20" s="4">
+        <v>17</v>
+      </c>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="O20" s="9">
+        <v>45</v>
+      </c>
+      <c r="P20" s="4">
+        <v>22</v>
+      </c>
+      <c r="Q20" s="9">
+        <v>40</v>
+      </c>
+      <c r="R20" s="4">
+        <v>19</v>
+      </c>
+      <c r="S20" s="18"/>
+      <c r="T20" s="18"/>
+      <c r="U20" s="18"/>
+      <c r="V20" s="18"/>
+      <c r="X20" s="18"/>
+      <c r="Y20" s="18"/>
+    </row>
+    <row r="21" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="10">
+        <v>42</v>
+      </c>
+      <c r="D21" s="6">
+        <v>13</v>
+      </c>
+      <c r="E21" s="10">
+        <v>38</v>
+      </c>
+      <c r="F21" s="6">
+        <v>38</v>
+      </c>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="O21" s="10">
+        <v>62</v>
+      </c>
+      <c r="P21" s="6">
+        <v>36</v>
+      </c>
+      <c r="Q21" s="10">
+        <v>47</v>
+      </c>
+      <c r="R21" s="6">
+        <v>18</v>
+      </c>
+      <c r="S21" s="18"/>
+      <c r="T21" s="18"/>
+      <c r="U21" s="18"/>
+      <c r="V21" s="18"/>
+    </row>
+    <row r="22" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="18"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="18"/>
+      <c r="N22" s="18"/>
+      <c r="O22" s="18"/>
+      <c r="P22" s="18"/>
+      <c r="Q22" s="18"/>
+      <c r="R22" s="18"/>
+      <c r="S22" s="18"/>
+      <c r="T22" s="18"/>
+      <c r="U22" s="18"/>
+      <c r="V22" s="18"/>
+    </row>
+    <row r="23" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="O23" s="20"/>
+      <c r="P23" s="20"/>
+      <c r="Q23" s="20"/>
+      <c r="R23" s="21"/>
+      <c r="S23" s="18"/>
+      <c r="T23" s="18"/>
+      <c r="U23" s="18"/>
+      <c r="V23" s="18"/>
+    </row>
+    <row r="24" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="14"/>
+      <c r="E24" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" s="14"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="O24" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="P24" s="14"/>
+      <c r="Q24" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="R24" s="14"/>
+      <c r="S24" s="18"/>
+      <c r="T24" s="18"/>
+      <c r="U24" s="18"/>
+      <c r="V24" s="18"/>
+    </row>
+    <row r="25" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="28"/>
+      <c r="C25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
+      <c r="M25" s="18"/>
+      <c r="N25" s="28"/>
+      <c r="O25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="R25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="S25" s="18"/>
+      <c r="T25" s="18"/>
+      <c r="U25" s="18"/>
+      <c r="V25" s="18"/>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="8">
+        <v>30</v>
+      </c>
+      <c r="D26" s="4">
+        <v>28</v>
+      </c>
+      <c r="E26" s="8">
+        <v>17</v>
+      </c>
+      <c r="F26" s="4">
+        <v>27</v>
+      </c>
+      <c r="H26" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="18"/>
+      <c r="N26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="O26" s="8">
+        <v>40</v>
+      </c>
+      <c r="P26" s="4">
+        <v>28</v>
+      </c>
+      <c r="Q26" s="8">
+        <v>22</v>
+      </c>
+      <c r="R26" s="4">
+        <v>16</v>
+      </c>
+      <c r="T26" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="U26" s="18"/>
+      <c r="V26" s="18"/>
+      <c r="W26" s="18"/>
+      <c r="X26" s="18"/>
+      <c r="Y26" s="18"/>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B27" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="9">
+        <v>96</v>
+      </c>
+      <c r="D27" s="4">
+        <v>26</v>
+      </c>
+      <c r="E27" s="9">
+        <v>98</v>
+      </c>
+      <c r="F27" s="4">
+        <v>29</v>
+      </c>
+      <c r="H27" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="18"/>
+      <c r="M27" s="18"/>
+      <c r="N27" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O27" s="9">
+        <v>94</v>
+      </c>
+      <c r="P27" s="4">
+        <v>15</v>
+      </c>
+      <c r="Q27" s="9">
+        <v>97</v>
+      </c>
+      <c r="R27" s="4">
+        <v>18</v>
+      </c>
+      <c r="T27" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="U27" s="18"/>
+      <c r="V27" s="18"/>
+      <c r="W27" s="18"/>
+      <c r="X27" s="18"/>
+      <c r="Y27" s="18"/>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="9">
+        <v>95</v>
+      </c>
+      <c r="D28" s="4">
+        <v>28</v>
+      </c>
+      <c r="E28" s="9">
+        <v>97</v>
+      </c>
+      <c r="F28" s="4">
+        <v>36</v>
+      </c>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="18"/>
+      <c r="M28" s="18"/>
+      <c r="N28" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="O28" s="9">
+        <v>94</v>
+      </c>
+      <c r="P28" s="4">
+        <v>16</v>
+      </c>
+      <c r="Q28" s="9">
+        <v>97</v>
+      </c>
+      <c r="R28" s="4">
+        <v>18</v>
+      </c>
+      <c r="S28" s="18"/>
+      <c r="T28" s="18"/>
+      <c r="U28" s="18"/>
+      <c r="V28" s="18"/>
+      <c r="X28" s="18"/>
+      <c r="Y28" s="18"/>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B29" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="9">
+        <v>32</v>
+      </c>
+      <c r="D29" s="4">
+        <v>28</v>
+      </c>
+      <c r="E29" s="9">
+        <v>18</v>
+      </c>
+      <c r="F29" s="4">
+        <v>28</v>
+      </c>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="18"/>
+      <c r="M29" s="18"/>
+      <c r="N29" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="O29" s="9">
+        <v>40</v>
+      </c>
+      <c r="P29" s="4">
+        <v>28</v>
+      </c>
+      <c r="Q29" s="9">
+        <v>22</v>
+      </c>
+      <c r="R29" s="4">
+        <v>16</v>
+      </c>
+      <c r="S29" s="18"/>
+      <c r="T29" s="18"/>
+      <c r="U29" s="18"/>
+      <c r="V29" s="18"/>
+    </row>
+    <row r="30" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="10">
+        <v>44</v>
+      </c>
+      <c r="D30" s="6">
+        <v>52</v>
+      </c>
+      <c r="E30" s="10">
+        <v>34</v>
+      </c>
+      <c r="F30" s="6">
+        <v>48</v>
+      </c>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="18"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="18"/>
+      <c r="M30" s="18"/>
+      <c r="N30" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="O30" s="10">
+        <v>50</v>
+      </c>
+      <c r="P30" s="6">
+        <v>28</v>
+      </c>
+      <c r="Q30" s="10">
+        <v>36</v>
+      </c>
+      <c r="R30" s="6">
+        <v>16</v>
+      </c>
+      <c r="S30" s="18"/>
+      <c r="T30" s="18"/>
+      <c r="U30" s="18"/>
+      <c r="V30" s="18"/>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="18"/>
+      <c r="L31" s="18"/>
+      <c r="M31" s="18"/>
+      <c r="N31" s="18"/>
+      <c r="O31" s="18"/>
+      <c r="P31" s="18"/>
+      <c r="Q31" s="18"/>
+      <c r="R31" s="18"/>
+      <c r="S31" s="18"/>
+      <c r="T31" s="18"/>
+      <c r="U31" s="18"/>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="18"/>
+      <c r="M32" s="18"/>
+      <c r="N32" s="18"/>
+      <c r="O32" s="18"/>
+      <c r="P32" s="18"/>
+      <c r="Q32" s="18"/>
+      <c r="R32" s="18"/>
+      <c r="S32" s="18"/>
+      <c r="T32" s="18"/>
+      <c r="U32" s="18"/>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A33" s="18"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="18"/>
+      <c r="M33" s="18"/>
+      <c r="N33" s="18"/>
+      <c r="O33" s="18"/>
+      <c r="P33" s="18"/>
+      <c r="Q33" s="18"/>
+      <c r="R33" s="18"/>
+      <c r="S33" s="18"/>
+      <c r="T33" s="18"/>
+      <c r="U33" s="18"/>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A34" s="18"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="18"/>
+      <c r="J34" s="18"/>
+      <c r="K34" s="18"/>
+      <c r="L34" s="18"/>
+      <c r="M34" s="18"/>
+      <c r="N34" s="18"/>
+      <c r="O34" s="18"/>
+      <c r="P34" s="18"/>
+      <c r="Q34" s="18"/>
+      <c r="R34" s="18"/>
+      <c r="S34" s="18"/>
+      <c r="T34" s="18"/>
+      <c r="U34" s="18"/>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A35" s="18"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="18"/>
+      <c r="I35" s="18"/>
+      <c r="J35" s="18"/>
+      <c r="K35" s="18"/>
+      <c r="L35" s="18"/>
+      <c r="M35" s="18"/>
+      <c r="N35" s="18"/>
+      <c r="O35" s="18"/>
+      <c r="P35" s="18"/>
+      <c r="Q35" s="18"/>
+      <c r="R35" s="18"/>
+      <c r="S35" s="18"/>
+      <c r="T35" s="18"/>
+      <c r="U35" s="18"/>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A36" s="18"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="18"/>
+      <c r="K36" s="18"/>
+      <c r="L36" s="18"/>
+      <c r="M36" s="18"/>
+      <c r="N36" s="18"/>
+      <c r="O36" s="18"/>
+      <c r="P36" s="18"/>
+      <c r="Q36" s="18"/>
+      <c r="R36" s="18"/>
+      <c r="S36" s="18"/>
+      <c r="T36" s="18"/>
+      <c r="U36" s="18"/>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A37" s="18"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="18"/>
+      <c r="J37" s="18"/>
+      <c r="K37" s="18"/>
+      <c r="L37" s="18"/>
+      <c r="M37" s="18"/>
+      <c r="N37" s="18"/>
+      <c r="O37" s="18"/>
+      <c r="P37" s="18"/>
+      <c r="Q37" s="18"/>
+      <c r="R37" s="18"/>
+      <c r="S37" s="18"/>
+      <c r="T37" s="18"/>
+      <c r="U37" s="18"/>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A38" s="18"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="18"/>
+      <c r="I38" s="18"/>
+      <c r="J38" s="18"/>
+      <c r="K38" s="18"/>
+      <c r="L38" s="18"/>
+      <c r="M38" s="18"/>
+      <c r="N38" s="18"/>
+      <c r="O38" s="18"/>
+      <c r="P38" s="18"/>
+      <c r="Q38" s="18"/>
+      <c r="R38" s="18"/>
+      <c r="S38" s="18"/>
+      <c r="T38" s="18"/>
+      <c r="U38" s="18"/>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A39" s="18"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="18"/>
+      <c r="I39" s="18"/>
+      <c r="J39" s="18"/>
+      <c r="K39" s="18"/>
+      <c r="L39" s="18"/>
+      <c r="M39" s="18"/>
+      <c r="N39" s="18"/>
+      <c r="O39" s="18"/>
+      <c r="P39" s="18"/>
+      <c r="Q39" s="18"/>
+      <c r="R39" s="18"/>
+      <c r="S39" s="18"/>
+      <c r="T39" s="18"/>
+      <c r="U39" s="18"/>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A40" s="18"/>
+      <c r="B40" s="18"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="18"/>
+      <c r="I40" s="18"/>
+      <c r="J40" s="18"/>
+      <c r="K40" s="18"/>
+      <c r="L40" s="18"/>
+      <c r="M40" s="18"/>
+      <c r="N40" s="18"/>
+      <c r="O40" s="18"/>
+      <c r="P40" s="18"/>
+      <c r="Q40" s="18"/>
+      <c r="R40" s="18"/>
+      <c r="S40" s="18"/>
+      <c r="T40" s="18"/>
+      <c r="U40" s="18"/>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A41" s="18"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="18"/>
+      <c r="I41" s="18"/>
+      <c r="J41" s="18"/>
+      <c r="K41" s="18"/>
+      <c r="L41" s="18"/>
+      <c r="M41" s="18"/>
+      <c r="N41" s="18"/>
+      <c r="O41" s="18"/>
+      <c r="P41" s="18"/>
+      <c r="Q41" s="18"/>
+      <c r="R41" s="18"/>
+      <c r="S41" s="18"/>
+      <c r="T41" s="18"/>
+      <c r="U41" s="18"/>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A42" s="18"/>
+      <c r="B42" s="18"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="18"/>
+      <c r="H42" s="18"/>
+      <c r="I42" s="18"/>
+      <c r="J42" s="18"/>
+      <c r="K42" s="18"/>
+      <c r="L42" s="18"/>
+      <c r="M42" s="18"/>
+      <c r="N42" s="18"/>
+      <c r="O42" s="18"/>
+      <c r="P42" s="18"/>
+      <c r="Q42" s="18"/>
+      <c r="R42" s="18"/>
+      <c r="S42" s="18"/>
+      <c r="T42" s="18"/>
+      <c r="U42" s="18"/>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A43" s="18"/>
+      <c r="B43" s="18"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="18"/>
+      <c r="G43" s="18"/>
+      <c r="H43" s="18"/>
+      <c r="I43" s="18"/>
+      <c r="J43" s="18"/>
+      <c r="K43" s="18"/>
+      <c r="L43" s="18"/>
+      <c r="M43" s="18"/>
+      <c r="N43" s="18"/>
+      <c r="O43" s="18"/>
+      <c r="P43" s="18"/>
+      <c r="Q43" s="18"/>
+      <c r="R43" s="18"/>
+      <c r="S43" s="18"/>
+      <c r="T43" s="18"/>
+      <c r="U43" s="18"/>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A44" s="18"/>
+      <c r="B44" s="18"/>
+      <c r="C44" s="26"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="18"/>
+      <c r="G44" s="18"/>
+      <c r="H44" s="18"/>
+      <c r="I44" s="18"/>
+      <c r="J44" s="18"/>
+      <c r="K44" s="18"/>
+      <c r="L44" s="18"/>
+      <c r="M44" s="18"/>
+      <c r="N44" s="18"/>
+      <c r="O44" s="18"/>
+      <c r="P44" s="18"/>
+      <c r="Q44" s="18"/>
+      <c r="R44" s="18"/>
+      <c r="S44" s="18"/>
+      <c r="T44" s="18"/>
+      <c r="U44" s="18"/>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A45" s="18"/>
+      <c r="B45" s="18"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="18"/>
+      <c r="H45" s="18"/>
+      <c r="I45" s="18"/>
+      <c r="J45" s="18"/>
+      <c r="K45" s="18"/>
+      <c r="L45" s="18"/>
+      <c r="M45" s="18"/>
+      <c r="N45" s="18"/>
+      <c r="O45" s="18"/>
+      <c r="P45" s="18"/>
+      <c r="Q45" s="18"/>
+      <c r="R45" s="18"/>
+      <c r="S45" s="18"/>
+      <c r="T45" s="18"/>
+      <c r="U45" s="18"/>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A46" s="18"/>
+      <c r="B46" s="18"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="18"/>
+      <c r="G46" s="18"/>
+      <c r="H46" s="18"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
+      <c r="K46" s="18"/>
+      <c r="L46" s="18"/>
+      <c r="M46" s="18"/>
+      <c r="N46" s="18"/>
+      <c r="O46" s="18"/>
+      <c r="P46" s="18"/>
+      <c r="Q46" s="18"/>
+      <c r="R46" s="18"/>
+      <c r="S46" s="18"/>
+      <c r="T46" s="18"/>
+      <c r="U46" s="18"/>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A47" s="18"/>
+      <c r="B47" s="18"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="18"/>
+      <c r="I47" s="18"/>
+      <c r="J47" s="18"/>
+      <c r="K47" s="18"/>
+      <c r="L47" s="18"/>
+      <c r="M47" s="18"/>
+      <c r="N47" s="18"/>
+      <c r="O47" s="18"/>
+      <c r="P47" s="18"/>
+      <c r="Q47" s="18"/>
+      <c r="R47" s="18"/>
+      <c r="S47" s="18"/>
+      <c r="T47" s="18"/>
+      <c r="U47" s="18"/>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A48" s="18"/>
+      <c r="B48" s="18"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
+      <c r="H48" s="18"/>
+      <c r="I48" s="18"/>
+      <c r="J48" s="18"/>
+      <c r="K48" s="18"/>
+      <c r="L48" s="18"/>
+      <c r="M48" s="18"/>
+      <c r="N48" s="18"/>
+      <c r="O48" s="18"/>
+      <c r="P48" s="18"/>
+      <c r="Q48" s="18"/>
+      <c r="R48" s="18"/>
+      <c r="S48" s="18"/>
+      <c r="T48" s="18"/>
+      <c r="U48" s="18"/>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A49" s="18"/>
+      <c r="B49" s="18"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="18"/>
+      <c r="G49" s="18"/>
+      <c r="H49" s="18"/>
+      <c r="I49" s="18"/>
+      <c r="J49" s="18"/>
+      <c r="K49" s="18"/>
+      <c r="L49" s="18"/>
+      <c r="M49" s="18"/>
+      <c r="N49" s="18"/>
+      <c r="O49" s="18"/>
+      <c r="P49" s="18"/>
+      <c r="Q49" s="18"/>
+      <c r="R49" s="18"/>
+      <c r="S49" s="18"/>
+      <c r="T49" s="18"/>
+      <c r="U49" s="18"/>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A50" s="18"/>
+      <c r="B50" s="18"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="18"/>
+      <c r="G50" s="18"/>
+      <c r="H50" s="18"/>
+      <c r="I50" s="18"/>
+      <c r="J50" s="18"/>
+      <c r="K50" s="18"/>
+      <c r="L50" s="18"/>
+      <c r="M50" s="18"/>
+      <c r="N50" s="18"/>
+      <c r="O50" s="18"/>
+      <c r="P50" s="18"/>
+      <c r="Q50" s="18"/>
+      <c r="R50" s="18"/>
+      <c r="S50" s="18"/>
+      <c r="T50" s="18"/>
+      <c r="U50" s="18"/>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A51" s="18"/>
+      <c r="B51" s="18"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="18"/>
+      <c r="G51" s="18"/>
+      <c r="H51" s="18"/>
+      <c r="I51" s="18"/>
+      <c r="J51" s="18"/>
+      <c r="K51" s="18"/>
+      <c r="L51" s="18"/>
+      <c r="M51" s="18"/>
+      <c r="N51" s="18"/>
+      <c r="O51" s="18"/>
+      <c r="P51" s="18"/>
+      <c r="Q51" s="18"/>
+      <c r="R51" s="18"/>
+      <c r="S51" s="18"/>
+      <c r="T51" s="18"/>
+      <c r="U51" s="18"/>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A52" s="18"/>
+      <c r="B52" s="18"/>
+      <c r="C52" s="18"/>
+      <c r="D52" s="18"/>
+      <c r="E52" s="18"/>
+      <c r="F52" s="18"/>
+      <c r="G52" s="18"/>
+      <c r="H52" s="18"/>
+      <c r="I52" s="18"/>
+      <c r="J52" s="18"/>
+      <c r="K52" s="18"/>
+      <c r="L52" s="18"/>
+      <c r="M52" s="18"/>
+      <c r="N52" s="18"/>
+      <c r="O52" s="18"/>
+      <c r="P52" s="18"/>
+      <c r="Q52" s="18"/>
+      <c r="R52" s="18"/>
+      <c r="S52" s="18"/>
+      <c r="T52" s="18"/>
+      <c r="U52" s="18"/>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B53" s="18"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="18"/>
+      <c r="I53" s="18"/>
+      <c r="J53" s="18"/>
+      <c r="K53" s="18"/>
+      <c r="L53" s="18"/>
+      <c r="M53" s="18"/>
+      <c r="N53" s="18"/>
+      <c r="O53" s="18"/>
+      <c r="P53" s="18"/>
+      <c r="Q53" s="18"/>
+      <c r="R53" s="18"/>
+      <c r="S53" s="18"/>
+      <c r="T53" s="18"/>
+      <c r="U53" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="24">
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="N23:R23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="N24:N25"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="N15:N16"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="N14:R14"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C6:D10">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E6:F10">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C17:D21">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C26:D30">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O17:P21">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O26:P30">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E17:F21">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E26:F30">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q17:R21">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q26:R30">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>